<commit_message>
fixxing bug with out of quota api
</commit_message>
<xml_diff>
--- a/log_data/temp.xlsx
+++ b/log_data/temp.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>first vids</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -458,17 +458,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V497.mp4</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\SEO_NO_LUC\Number SLime\440HBB.mp4</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>60</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V497_Tuan_number_ghep.mp4</t>
+          <t>D:\Output\Number\440HBB_Number.mp4</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -480,17 +478,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V496 - Hải chú ý giảm sáng.mp4</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\SEO_NO_LUC\Number SLime\436HBD.mp4</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>60</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V496 - Hải chú ý giảm sáng_Tuan_number_ghep.mp4</t>
+          <t>D:\Output\Number\436HBD_Number.mp4</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -502,19 +498,13 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V493.mp4</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>D:\Output\Thomas\V493_Tuan_number_ghep.mp4</t>
-        </is>
-      </c>
+          <t>\\SEO_NO_LUC\Number\Number A\Video\456GLD.mp4</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>60</v>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>Done</t>
@@ -524,17 +514,15 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V492.mp4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\SEO_NO_LUC\Number\Number A\Video\472GLD.mp4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>60</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V492_Thomas.mp4</t>
+          <t>D:\Output\Number\472GLD_Number.mp4</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -546,17 +534,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V486.mp4</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\SEO_NO_LUC\Number SLime\442DBB.mp4</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>60</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V486_Thomas.mp4</t>
+          <t>D:\Output\Number\442DBB_Number.mp4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -568,17 +554,15 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V485-new.mp4</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\SEO_NO_LUC\Number SLime\439HBB.mp4</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>60</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V485-new_Thomas.mp4</t>
+          <t>D:\Output\Number\439HBB_Number.mp4</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -590,17 +574,15 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V484.mp4</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\SEO_NO_LUC\Number\Number A\Video\486HDD.mp4</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>60</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V484_Thomas.mp4</t>
+          <t>D:\Output\Number\486HDD_Number.mp4</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -612,17 +594,15 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V483.mp4</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\SEO_NO_LUC\Number SLime\443DBD.mp4</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>60</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V483_Thomas.mp4</t>
+          <t>D:\Output\Number\443DBD_Number.mp4</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -634,17 +614,15 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V482.mp4</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\SEO_NO_LUC\Number SLime\441DBB.mp4</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>60</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V482_Thomas.mp4</t>
+          <t>D:\Output\Number\441DBB_Number.mp4</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -656,17 +634,15 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V481.mp4</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\seo_no_luc\Number\Number A\Video\546DBF.mp4</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>90</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V481_Thomas.mp4</t>
+          <t>D:\Output\Number\546DBF_Number.mp4</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -678,17 +654,15 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V480.mp4</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\seo_no_luc\Number\Number A\Video\351HLA.mp4</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>60</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V480_Thomas.mp4</t>
+          <t>D:\Output\Number\351HLA_Number.mp4</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -700,17 +674,15 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V479.mp4</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\seo_no_luc\Number\Rainbow Number\Video\40FBA.mp4</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>60</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V479_Thomas.mp4</t>
+          <t>D:\Output\Number\40FBA_Number.mp4</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -722,17 +694,15 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V478.mp4</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\seo_no_luc\Number\Number A\Video\553DDF.mp4</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>90</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V478_Thomas.mp4</t>
+          <t>D:\Output\Number\553DDF_Number.mp4</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -744,17 +714,15 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V477.mp4</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\seo_no_luc\Number\Number A\Video\363HLC.mp4</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>60</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V477_Thomas.mp4</t>
+          <t>D:\Output\Number\363HLC_Number.mp4</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -766,17 +734,15 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V476.mp4</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>\\seo_no_luc\Number\Rainbow Number\Video\467KB.mp4</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>60</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V476_Thomas.mp4</t>
+          <t>D:\Output\Number\467KB_Number.mp4</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -788,17 +754,15 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V471-sua1.mp4</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+          <t>\\seo_no_luc\Number\Number A\Video\426KLE.mp4</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>90</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V471-sua1_Thomas.mp4</t>
+          <t>D:\Output\Number\426KLE_Number.mp4</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -810,17 +774,15 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V475.mp4</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+          <t>\\seo_no_luc\Number\Number B\Video\450HBB.mp4</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>60</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V475_Thomas.mp4</t>
+          <t>D:\Output\Number\450HBB_Number.mp4</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -832,17 +794,15 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V474.mp4</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+          <t>\\seo_no_luc\Number\Rainbow Number\Video\37FBA.mp4</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>60</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V474_Thomas.mp4</t>
+          <t>D:\Output\Number\37FBA_Number.mp4</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -854,17 +814,15 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V473-sua.mp4</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+          <t>\\seo_no_luc\Number\Number A\Video\558DDD.mp4</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>90</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V473-sua_Thomas.mp4</t>
+          <t>D:\Output\Number\558DDD_Number.mp4</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -876,20 +834,1418 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>\\seo_no_luc\Unboxing doll\Thomas\V472-sua.mp4</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+          <t>\\seo_no_luc\Number\Number B\Video\348KCC-Hiếu.mp4</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>60</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>D:\Output\Thomas\V472-sua_Thomas.mp4</t>
+          <t>D:\Output\Number\348KCC-Hiếu_Number.mp4</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>\\seo_no_luc\Number\Rainbow Number\Video\39FBA.mp4</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>60</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\39FBA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>\\seo_no_luc\Number\Number A\Video\484GLD.mp4</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>90</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\484GLD_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>\\seo_no_luc\Number\Number A\Video\390BGA.mp4</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>60</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\390BGA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>\\seo_no_luc\Number\Rainbow Number\Video\449HB.mp4</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>60</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\449HB_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>\\seo_no_luc\Number\Number A\Video\560HBF.mp4</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>90</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\560HBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>\\seo_no_luc\Number\Number A\Video\482GDC.mp4</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>60</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\482GDC_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>\\seo_no_luc\Number\Rainbow Number\Video\61GB-7B.mp4</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>60</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\61GB-7B_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>\\seo_no_luc\Number\Number A\Video\562HBF.mp4</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>90</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\562HBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>\\seo_no_luc\Number\Number A\Video\364HLC.mp4</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>60</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\364HLC_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>\\seo_no_luc\Number\Number TC\Video\27AE.mp4</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>60</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\27AE_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\462KBF.mp4</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>60</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\462KBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number\Number SLime\Video\257HLA.mp4</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>60</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\257HLA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\461KBF.mp4</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>60</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\461KBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\461KBF.mp4</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>60</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\461KBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\444DBF.mp4</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>58</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\444DBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number\Rainbow Number\Video\385GC.mp4</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>58</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\385GC_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\Video\461KBF.mp4</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>58</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\461KBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\445DBF.mp4</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>59</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\445DBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\570KBD.mp4"</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>90</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\570KBD_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\170BGB_1.mp4"</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>90</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\170BGB_1_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\466KBB.mp4"</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>60</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\466KBB_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number SLime\Video\250KLA.mp4"</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>60</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\250KLA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number SLime\Video\393HDA.mp4"</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>90</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\393HDA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\468KBB.mp4"</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>60</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\468KBB_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number SLime\Video\253GLC.mp4"</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>60</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\253GLC_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\464HBE.mp4"</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>90</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\464HBE_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\356GLA.mp4"</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>60</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\356GLA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\467KBB.mp4"</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>60</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\467KBB_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number SLime\Video\257HLA.mp4"</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>60</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\257HLA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\38BFA.mp4"</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>60</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\38BFA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\161BA.mp4"</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>90</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\161BA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\456DDD.mp4</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>60</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\456DDD_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\Video\463KBE.mp4</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>60</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\463KBE_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\388BKG.mp4"</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>90</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\388BKG_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\538GBB.mp4"</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>90</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\538GBB_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number SLime\Video\258HLA.mp4"</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>60</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\258HLA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number SLime\Video\259HLA.mp4"</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>60</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\259HLA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\316KLG.mp4"</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>60</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\316KLG_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\339GBC.mp4"</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>60</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\339GBC_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\292KLD.mp4"</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>60</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\292KLD_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number\Number A\Video\114FC.mp4</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>59</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\114FC_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number\Number A\Video\348GLA.mp4</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>59</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\348GLA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\561HBF.mp4"</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>90</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\561HBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\464KBE.mp4</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>60</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\464KBE_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number\Number SLime\Video\387KLD.mp4</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>59</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\387KLD_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\473KBB.mp4"</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>60</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\473KBB_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\459DDF.mp4</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>58</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\459DDF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\566HBF.mp4"</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>90</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\566HBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\469KBB.mp4"</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>60</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\469KBB_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Rainbow Number\Video\450HB.mp4"</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>60</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\450HB_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\565DBF.mp4"</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>90</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\565DBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\471KBB.mp4"</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>60</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\471KBB_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Rainbow Number\Video\435HB.mp4"</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>60</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\435HB_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\515KBF.mp4"</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>90</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\515KBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\101BGA.mp4"</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>60</v>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\101BGA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Rainbow Number\Video\V130FD.mp4"</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>60</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\V130FD_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\556DDD.mp4"</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>90</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\556DDD_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\472KBB.mp4"</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>60</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\472KBB_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Rainbow Number\Video\337HE - 345A sua lai.mp4"</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>60</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\337HE - 345A sua lai_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\345HAD.mp4"</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>90</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\345HAD_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\112BGA.mp4"</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>60</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\112BGA_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number SLime\Video\390HLD.mp4"</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>60</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\390HLD_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Rainbow Number\Video\358HE - 300A.mp4"</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>60</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\358HE - 300A_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Rainbow Number\Video\357HE - 299A.mp4"</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>60</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Ghép video hoàn tất: D:\Output\Number\357HE - 299A_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\Video\409GLB.mp4</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>59</v>
+      </c>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\469KBF.mp4</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>60</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\469KBF_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>\\SEO_NO_LUC\Number SLime\468KBD.mp4</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>58</v>
+      </c>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\581DBF.mp4"</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>90</v>
+      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number A\Video\578KBF.mp4"</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>90</v>
+      </c>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>"\\seo_no_luc\Number\Number B\Video\377HBF.mp4"</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>60</v>
+      </c>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>"C:\Users\Seo no luc\Documents\dev\test\test.mp4"</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>5</v>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\test_Number.mp4</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
         <is>
           <t>Done</t>
         </is>

</xml_diff>

<commit_message>
update select 3 videos
</commit_message>
<xml_diff>
--- a/log_data/temp.xlsx
+++ b/log_data/temp.xlsx
@@ -473,10 +473,8 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D2" t="n">
+        <v>60</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -497,10 +495,8 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D3" t="n">
+        <v>60</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -521,10 +517,8 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D4" t="n">
+        <v>60</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
@@ -541,10 +535,8 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D5" t="n">
+        <v>60</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -565,10 +557,8 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D6" t="n">
+        <v>60</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -589,10 +579,8 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D7" t="n">
+        <v>60</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -613,10 +601,8 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D8" t="n">
+        <v>60</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -637,10 +623,8 @@
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D9" t="n">
+        <v>60</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -661,10 +645,8 @@
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D10" t="n">
+        <v>60</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -685,10 +667,8 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D11" t="n">
+        <v>90</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -709,10 +689,8 @@
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D12" t="n">
+        <v>60</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -733,10 +711,8 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D13" t="n">
+        <v>60</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -757,10 +733,8 @@
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D14" t="n">
+        <v>90</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -781,10 +755,8 @@
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D15" t="n">
+        <v>60</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -805,10 +777,8 @@
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D16" t="n">
+        <v>60</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -829,10 +799,8 @@
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D17" t="n">
+        <v>90</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -853,10 +821,8 @@
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D18" t="n">
+        <v>60</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -877,10 +843,8 @@
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D19" t="n">
+        <v>60</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -901,10 +865,8 @@
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D20" t="n">
+        <v>90</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -925,10 +887,8 @@
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D21" t="n">
+        <v>60</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -949,10 +909,8 @@
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D22" t="n">
+        <v>60</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -973,10 +931,8 @@
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D23" t="n">
+        <v>90</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -997,10 +953,8 @@
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D24" t="n">
+        <v>60</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1021,10 +975,8 @@
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D25" t="n">
+        <v>60</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1045,10 +997,8 @@
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D26" t="n">
+        <v>90</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1069,10 +1019,8 @@
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D27" t="n">
+        <v>60</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1093,10 +1041,8 @@
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D28" t="n">
+        <v>60</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1117,10 +1063,8 @@
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D29" t="n">
+        <v>90</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1141,10 +1085,8 @@
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D30" t="n">
+        <v>60</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1165,10 +1107,8 @@
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D31" t="n">
+        <v>60</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1189,10 +1129,8 @@
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D32" t="n">
+        <v>60</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1213,10 +1151,8 @@
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D33" t="n">
+        <v>60</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1237,10 +1173,8 @@
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D34" t="n">
+        <v>60</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1261,10 +1195,8 @@
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D35" t="n">
+        <v>60</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1285,10 +1217,8 @@
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="D36" t="n">
+        <v>58</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1309,10 +1239,8 @@
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr"/>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="D37" t="n">
+        <v>58</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1333,10 +1261,8 @@
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="D38" t="n">
+        <v>58</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1357,10 +1283,8 @@
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+      <c r="D39" t="n">
+        <v>59</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1381,10 +1305,8 @@
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr"/>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D40" t="n">
+        <v>90</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1405,10 +1327,8 @@
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr"/>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D41" t="n">
+        <v>90</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1429,10 +1349,8 @@
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D42" t="n">
+        <v>60</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1453,10 +1371,8 @@
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D43" t="n">
+        <v>60</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1477,10 +1393,8 @@
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr"/>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D44" t="n">
+        <v>90</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1501,10 +1415,8 @@
       </c>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D45" t="n">
+        <v>60</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1525,10 +1437,8 @@
       </c>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D46" t="n">
+        <v>60</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1549,10 +1459,8 @@
       </c>
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D47" t="n">
+        <v>90</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1573,10 +1481,8 @@
       </c>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr"/>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D48" t="n">
+        <v>60</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1597,10 +1503,8 @@
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D49" t="n">
+        <v>60</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1621,10 +1525,8 @@
       </c>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D50" t="n">
+        <v>60</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1645,10 +1547,8 @@
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D51" t="n">
+        <v>60</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1669,10 +1569,8 @@
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr"/>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D52" t="n">
+        <v>90</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1693,10 +1591,8 @@
       </c>
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D53" t="n">
+        <v>60</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1717,10 +1613,8 @@
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D54" t="n">
+        <v>60</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1741,10 +1635,8 @@
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D55" t="n">
+        <v>90</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1765,10 +1657,8 @@
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D56" t="n">
+        <v>90</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1789,10 +1679,8 @@
       </c>
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D57" t="n">
+        <v>60</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1813,10 +1701,8 @@
       </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D58" t="n">
+        <v>60</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1837,10 +1723,8 @@
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D59" t="n">
+        <v>60</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1861,10 +1745,8 @@
       </c>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D60" t="n">
+        <v>60</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1885,10 +1767,8 @@
       </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D61" t="n">
+        <v>60</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1909,10 +1789,8 @@
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+      <c r="D62" t="n">
+        <v>59</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1933,10 +1811,8 @@
       </c>
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+      <c r="D63" t="n">
+        <v>59</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -1957,10 +1833,8 @@
       </c>
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D64" t="n">
+        <v>90</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -1981,10 +1855,8 @@
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D65" t="n">
+        <v>60</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2005,10 +1877,8 @@
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+      <c r="D66" t="n">
+        <v>59</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2029,10 +1899,8 @@
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D67" t="n">
+        <v>60</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2053,10 +1921,8 @@
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="D68" t="n">
+        <v>58</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2077,10 +1943,8 @@
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D69" t="n">
+        <v>90</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2101,10 +1965,8 @@
       </c>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D70" t="n">
+        <v>60</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2125,10 +1987,8 @@
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D71" t="n">
+        <v>60</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2149,10 +2009,8 @@
       </c>
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D72" t="n">
+        <v>90</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2173,10 +2031,8 @@
       </c>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D73" t="n">
+        <v>60</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2197,10 +2053,8 @@
       </c>
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D74" t="n">
+        <v>60</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2221,10 +2075,8 @@
       </c>
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D75" t="n">
+        <v>90</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2245,10 +2097,8 @@
       </c>
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D76" t="n">
+        <v>60</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2269,10 +2119,8 @@
       </c>
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D77" t="n">
+        <v>60</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2293,10 +2141,8 @@
       </c>
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D78" t="n">
+        <v>90</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2317,10 +2163,8 @@
       </c>
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr"/>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D79" t="n">
+        <v>60</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2341,10 +2185,8 @@
       </c>
       <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D80" t="n">
+        <v>60</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2365,10 +2207,8 @@
       </c>
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D81" t="n">
+        <v>90</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2389,10 +2229,8 @@
       </c>
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr"/>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D82" t="n">
+        <v>60</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2413,10 +2251,8 @@
       </c>
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr"/>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D83" t="n">
+        <v>60</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2437,10 +2273,8 @@
       </c>
       <c r="B84" t="inlineStr"/>
       <c r="C84" t="inlineStr"/>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D84" t="n">
+        <v>60</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2461,10 +2295,8 @@
       </c>
       <c r="B85" t="inlineStr"/>
       <c r="C85" t="inlineStr"/>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D85" t="n">
+        <v>60</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2485,10 +2317,8 @@
       </c>
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr"/>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>59</t>
-        </is>
+      <c r="D86" t="n">
+        <v>59</v>
       </c>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr">
@@ -2505,10 +2335,8 @@
       </c>
       <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr"/>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D87" t="n">
+        <v>60</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2529,10 +2357,8 @@
       </c>
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="D88" t="n">
+        <v>58</v>
       </c>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr">
@@ -2549,10 +2375,8 @@
       </c>
       <c r="B89" t="inlineStr"/>
       <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D89" t="n">
+        <v>90</v>
       </c>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr">
@@ -2569,10 +2393,8 @@
       </c>
       <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D90" t="n">
+        <v>90</v>
       </c>
       <c r="E90" t="inlineStr"/>
       <c r="F90" t="inlineStr">
@@ -2589,10 +2411,8 @@
       </c>
       <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr"/>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D91" t="n">
+        <v>60</v>
       </c>
       <c r="E91" t="inlineStr"/>
       <c r="F91" t="inlineStr">
@@ -2609,10 +2429,8 @@
       </c>
       <c r="B92" t="inlineStr"/>
       <c r="C92" t="inlineStr"/>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="D92" t="n">
+        <v>5</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2633,10 +2451,8 @@
       </c>
       <c r="B93" t="inlineStr"/>
       <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>70</t>
-        </is>
+      <c r="D93" t="n">
+        <v>70</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2657,10 +2473,8 @@
       </c>
       <c r="B94" t="inlineStr"/>
       <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D94" t="n">
+        <v>60</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2681,10 +2495,8 @@
       </c>
       <c r="B95" t="inlineStr"/>
       <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
+      <c r="D95" t="n">
+        <v>58</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2705,10 +2517,8 @@
       </c>
       <c r="B96" t="inlineStr"/>
       <c r="C96" t="inlineStr"/>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D96" t="n">
+        <v>60</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2729,10 +2539,8 @@
       </c>
       <c r="B97" t="inlineStr"/>
       <c r="C97" t="inlineStr"/>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D97" t="n">
+        <v>90</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2753,10 +2561,8 @@
       </c>
       <c r="B98" t="inlineStr"/>
       <c r="C98" t="inlineStr"/>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D98" t="n">
+        <v>60</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2777,10 +2583,8 @@
       </c>
       <c r="B99" t="inlineStr"/>
       <c r="C99" t="inlineStr"/>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D99" t="n">
+        <v>60</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2801,10 +2605,8 @@
       </c>
       <c r="B100" t="inlineStr"/>
       <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D100" t="n">
+        <v>90</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2825,10 +2627,8 @@
       </c>
       <c r="B101" t="inlineStr"/>
       <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D101" t="n">
+        <v>60</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2849,10 +2649,8 @@
       </c>
       <c r="B102" t="inlineStr"/>
       <c r="C102" t="inlineStr"/>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D102" t="n">
+        <v>60</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2873,10 +2671,8 @@
       </c>
       <c r="B103" t="inlineStr"/>
       <c r="C103" t="inlineStr"/>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D103" t="n">
+        <v>90</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -2897,10 +2693,8 @@
       </c>
       <c r="B104" t="inlineStr"/>
       <c r="C104" t="inlineStr"/>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D104" t="n">
+        <v>60</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -2921,10 +2715,8 @@
       </c>
       <c r="B105" t="inlineStr"/>
       <c r="C105" t="inlineStr"/>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D105" t="n">
+        <v>60</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -2945,10 +2737,8 @@
       </c>
       <c r="B106" t="inlineStr"/>
       <c r="C106" t="inlineStr"/>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D106" t="n">
+        <v>60</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -2969,10 +2759,8 @@
       </c>
       <c r="B107" t="inlineStr"/>
       <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D107" t="n">
+        <v>60</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -2993,10 +2781,8 @@
       </c>
       <c r="B108" t="inlineStr"/>
       <c r="C108" t="inlineStr"/>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D108" t="n">
+        <v>90</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3017,10 +2803,8 @@
       </c>
       <c r="B109" t="inlineStr"/>
       <c r="C109" t="inlineStr"/>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D109" t="n">
+        <v>90</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3041,10 +2825,8 @@
       </c>
       <c r="B110" t="inlineStr"/>
       <c r="C110" t="inlineStr"/>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D110" t="n">
+        <v>60</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3065,10 +2847,8 @@
       </c>
       <c r="B111" t="inlineStr"/>
       <c r="C111" t="inlineStr"/>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D111" t="n">
+        <v>60</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3089,10 +2869,8 @@
       </c>
       <c r="B112" t="inlineStr"/>
       <c r="C112" t="inlineStr"/>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>60</t>
-        </is>
+      <c r="D112" t="n">
+        <v>60</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3113,10 +2891,8 @@
       </c>
       <c r="B113" t="inlineStr"/>
       <c r="C113" t="inlineStr"/>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+      <c r="D113" t="n">
+        <v>40</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3137,10 +2913,8 @@
       </c>
       <c r="B114" t="inlineStr"/>
       <c r="C114" t="inlineStr"/>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>45</t>
-        </is>
+      <c r="D114" t="n">
+        <v>45</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3161,10 +2935,8 @@
       </c>
       <c r="B115" t="inlineStr"/>
       <c r="C115" t="inlineStr"/>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>63</t>
-        </is>
+      <c r="D115" t="n">
+        <v>63</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3185,10 +2957,8 @@
       </c>
       <c r="B116" t="inlineStr"/>
       <c r="C116" t="inlineStr"/>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
+      <c r="D116" t="n">
+        <v>61</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3209,10 +2979,8 @@
       </c>
       <c r="B117" t="inlineStr"/>
       <c r="C117" t="inlineStr"/>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D117" t="n">
+        <v>90</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3233,10 +3001,8 @@
       </c>
       <c r="B118" t="inlineStr"/>
       <c r="C118" t="inlineStr"/>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t>90</t>
-        </is>
+      <c r="D118" t="n">
+        <v>90</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3255,25 +3021,20 @@
           <t>"C:\Users\Seo no luc\Documents\test.mp4"</t>
         </is>
       </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>"C:\Users\Seo no luc\Documents\test.mp4"</t>
-        </is>
-      </c>
-      <c r="C119" t="inlineStr">
-        <is>
-          <t>"C:\Users\Seo no luc\Documents\test.mp4"</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="E119" t="inlineStr"/>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="n">
+        <v>3</v>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>D:\Output\Number\test_Number.mp4
+D:\Output\Number\test_Number.mp4</t>
+        </is>
+      </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Auto</t>
+          <t>Done</t>
         </is>
       </c>
     </row>

</xml_diff>